<commit_message>
Made tests fail correctly
</commit_message>
<xml_diff>
--- a/ClueBoard.xlsx
+++ b/ClueBoard.xlsx
@@ -16,32 +16,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="37">
   <si>
     <t>E</t>
   </si>
   <si>
-    <t xml:space="preserve">E = </t>
-  </si>
-  <si>
     <t>Entryway</t>
   </si>
   <si>
     <t>A</t>
   </si>
   <si>
-    <t>A =</t>
-  </si>
-  <si>
     <t>Armory</t>
   </si>
   <si>
     <t>B</t>
   </si>
   <si>
-    <t>B =</t>
-  </si>
-  <si>
     <t>Barracks</t>
   </si>
   <si>
@@ -51,33 +42,21 @@
     <t>S</t>
   </si>
   <si>
-    <t>L =</t>
-  </si>
-  <si>
     <t>O</t>
   </si>
   <si>
     <t>G</t>
   </si>
   <si>
-    <t>G =</t>
-  </si>
-  <si>
     <t>Great Hall</t>
   </si>
   <si>
     <t>T</t>
   </si>
   <si>
-    <t>T =</t>
-  </si>
-  <si>
     <t>Throne Room</t>
   </si>
   <si>
-    <t>O =</t>
-  </si>
-  <si>
     <t>Oubliette</t>
   </si>
   <si>
@@ -93,12 +72,6 @@
     <t>Dungeon</t>
   </si>
   <si>
-    <t>D =</t>
-  </si>
-  <si>
-    <t>S =</t>
-  </si>
-  <si>
     <t>Solar</t>
   </si>
   <si>
@@ -108,15 +81,9 @@
     <t>K</t>
   </si>
   <si>
-    <t>K =</t>
-  </si>
-  <si>
     <t>Kitchen</t>
   </si>
   <si>
-    <t>C =</t>
-  </si>
-  <si>
     <t>Chapel</t>
   </si>
   <si>
@@ -156,10 +123,10 @@
     <t>AU</t>
   </si>
   <si>
-    <t>X =</t>
-  </si>
-  <si>
     <t>X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E </t>
   </si>
 </sst>
 </file>
@@ -562,7 +529,7 @@
   <dimension ref="A1:AC26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+      <selection activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,1551 +540,1551 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="Z3" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC4" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="X6" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="Z6" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="S7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="U7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="W7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="X7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z7" s="6" t="s">
-        <v>39</v>
-      </c>
       <c r="AB7" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="AC7" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W8" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Y8" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Z8" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="AB8" s="2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="AC8" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="V9" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W9" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X9" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y9" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z9" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="U10" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="V10" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W10" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X10" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y10" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z10" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="U11" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="V11" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W11" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X11" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y11" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z11" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AB11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC11" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="AC11" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="S12" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="T12" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W12" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X12" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y12" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z12" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AB12" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="AC12" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="T13" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="U13" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W13" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X13" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y13" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z13" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AB13" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="AC13" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q14" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="R14" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="S14" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="T14" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="U14" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="V14" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W14" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X14" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y14" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z14" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AB14" s="3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="AC14" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="K15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="R15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="S15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="U15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="V15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="W15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="X15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC15" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q15" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="R15" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="S15" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="T15" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="U15" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="V15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="W15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="X15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC15" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q16" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="R16" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="S16" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="T16" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="U16" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="V16" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W16" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X16" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y16" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z16" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="P17" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q17" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="R17" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="S17" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="T17" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="U17" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="V17" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W17" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X17" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y17" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z17" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="P18" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q18" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="R18" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="S18" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="T18" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="U18" s="8" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="V18" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W18" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X18" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y18" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z18" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L19" s="4" t="s">
         <v>0</v>
@@ -2129,75 +2096,75 @@
         <v>0</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="P19" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="R19" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="S19" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="T19" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="U19" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="V19" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W19" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X19" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y19" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z19" s="9" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>0</v>
@@ -2209,75 +2176,75 @@
         <v>0</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S20" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="T20" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U20" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V20" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W20" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="X20" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Y20" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Z20" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>0</v>
@@ -2289,75 +2256,75 @@
         <v>0</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="P21" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S21" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="T21" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U21" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V21" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W21" s="6" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="X21" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="Y21" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Z21" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>0</v>
@@ -2369,75 +2336,75 @@
         <v>0</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S22" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="T22" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U22" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V22" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W22" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="X22" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="Y22" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Z22" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>0</v>
@@ -2449,75 +2416,75 @@
         <v>0</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="P23" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="R23" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S23" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="T23" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U23" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V23" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W23" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="X23" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="Y23" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="Z23" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L24" s="4" t="s">
         <v>0</v>
@@ -2529,75 +2496,75 @@
         <v>0</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U24" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V24" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W24" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="X24" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="Y24" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="Z24" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>0</v>
@@ -2609,75 +2576,75 @@
         <v>0</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="P25" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q25" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="R25" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S25" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="T25" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U25" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V25" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W25" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="X25" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="Y25" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="Z25" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="L26" s="4" t="s">
         <v>0</v>
@@ -2689,40 +2656,40 @@
         <v>0</v>
       </c>
       <c r="O26" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="P26" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q26" s="6" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="R26" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S26" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="T26" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U26" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V26" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="W26" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="X26" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="Y26" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="Z26" s="4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished loadBoardConfig method, just needs to be cleaned up a bit
</commit_message>
<xml_diff>
--- a/ClueBoard.xlsx
+++ b/ClueBoard.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="38">
   <si>
     <t>E</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t xml:space="preserve">E </t>
+  </si>
+  <si>
+    <t>Walkway</t>
   </si>
 </sst>
 </file>
@@ -187,7 +190,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -210,11 +213,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -225,6 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,7 +544,7 @@
   <dimension ref="A1:AC26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB15" sqref="AB15"/>
+      <selection activeCell="AC16" sqref="AB4:AC16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,6 +1905,12 @@
       </c>
       <c r="Z16" s="7" t="s">
         <v>4</v>
+      </c>
+      <c r="AB16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC16" s="10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Made some more tests pass
</commit_message>
<xml_diff>
--- a/ClueBoard.xlsx
+++ b/ClueBoard.xlsx
@@ -541,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC26"/>
+  <dimension ref="A1:AC27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC16" sqref="AB4:AC16"/>
+      <selection activeCell="Z28" sqref="Z28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,6 +632,9 @@
       <c r="Z1" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="AA1">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -712,6 +715,9 @@
       <c r="Z2" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -791,6 +797,9 @@
       </c>
       <c r="Z3" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="AA3">
+        <v>2</v>
       </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
@@ -874,6 +883,9 @@
       <c r="Z4" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="AA4">
+        <v>3</v>
+      </c>
       <c r="AB4" s="2" t="s">
         <v>19</v>
       </c>
@@ -960,6 +972,9 @@
       <c r="Z5" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="AA5">
+        <v>4</v>
+      </c>
       <c r="AB5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1046,6 +1061,9 @@
       <c r="Z6" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="AA6">
+        <v>5</v>
+      </c>
       <c r="AB6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1132,6 +1150,9 @@
       <c r="Z7" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="AA7">
+        <v>6</v>
+      </c>
       <c r="AB7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1218,6 +1239,9 @@
       <c r="Z8" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="AA8">
+        <v>7</v>
+      </c>
       <c r="AB8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1304,6 +1328,9 @@
       <c r="Z9" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="AA9">
+        <v>8</v>
+      </c>
       <c r="AB9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1390,6 +1417,9 @@
       <c r="Z10" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="AA10">
+        <v>9</v>
+      </c>
       <c r="AB10" s="2" t="s">
         <v>4</v>
       </c>
@@ -1476,6 +1506,9 @@
       <c r="Z11" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="AA11">
+        <v>10</v>
+      </c>
       <c r="AB11" s="2" t="s">
         <v>36</v>
       </c>
@@ -1561,6 +1594,9 @@
       </c>
       <c r="Z12" s="7" t="s">
         <v>4</v>
+      </c>
+      <c r="AA12">
+        <v>11</v>
       </c>
       <c r="AB12" s="3" t="s">
         <v>9</v>
@@ -1648,6 +1684,9 @@
       <c r="Z13" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="AA13">
+        <v>12</v>
+      </c>
       <c r="AB13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1734,6 +1773,9 @@
       <c r="Z14" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="AA14">
+        <v>13</v>
+      </c>
       <c r="AB14" s="3" t="s">
         <v>8</v>
       </c>
@@ -1820,6 +1862,9 @@
       <c r="Z15" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="AA15">
+        <v>14</v>
+      </c>
       <c r="AB15" s="3" t="s">
         <v>35</v>
       </c>
@@ -1906,6 +1951,9 @@
       <c r="Z16" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="AA16">
+        <v>15</v>
+      </c>
       <c r="AB16" s="10" t="s">
         <v>15</v>
       </c>
@@ -1913,7 +1961,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -1992,8 +2040,11 @@
       <c r="Z17" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="AA17">
+        <v>16</v>
+      </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
@@ -2072,8 +2123,11 @@
       <c r="Z18" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="AA18">
+        <v>17</v>
+      </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>8</v>
       </c>
@@ -2152,8 +2206,11 @@
       <c r="Z19" s="9" t="s">
         <v>29</v>
       </c>
+      <c r="AA19">
+        <v>18</v>
+      </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>8</v>
       </c>
@@ -2232,8 +2289,11 @@
       <c r="Z20" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="AA20">
+        <v>19</v>
+      </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
@@ -2312,8 +2372,11 @@
       <c r="Z21" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="AA21">
+        <v>20</v>
+      </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>8</v>
       </c>
@@ -2392,8 +2455,11 @@
       <c r="Z22" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="AA22">
+        <v>21</v>
+      </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>8</v>
       </c>
@@ -2472,8 +2538,11 @@
       <c r="Z23" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="AA23">
+        <v>22</v>
+      </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>8</v>
       </c>
@@ -2552,8 +2621,11 @@
       <c r="Z24" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="AA24">
+        <v>23</v>
+      </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>8</v>
       </c>
@@ -2632,8 +2704,11 @@
       <c r="Z25" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="AA25">
+        <v>24</v>
+      </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>8</v>
       </c>
@@ -2711,6 +2786,89 @@
       </c>
       <c r="Z26" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="AA26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>5</v>
+      </c>
+      <c r="G27">
+        <v>6</v>
+      </c>
+      <c r="H27">
+        <v>7</v>
+      </c>
+      <c r="I27">
+        <v>8</v>
+      </c>
+      <c r="J27">
+        <v>9</v>
+      </c>
+      <c r="K27">
+        <v>10</v>
+      </c>
+      <c r="L27">
+        <v>11</v>
+      </c>
+      <c r="M27">
+        <v>12</v>
+      </c>
+      <c r="N27">
+        <v>13</v>
+      </c>
+      <c r="O27">
+        <v>14</v>
+      </c>
+      <c r="P27">
+        <v>15</v>
+      </c>
+      <c r="Q27">
+        <v>16</v>
+      </c>
+      <c r="R27">
+        <v>17</v>
+      </c>
+      <c r="S27">
+        <v>18</v>
+      </c>
+      <c r="T27">
+        <v>19</v>
+      </c>
+      <c r="U27">
+        <v>20</v>
+      </c>
+      <c r="V27">
+        <v>21</v>
+      </c>
+      <c r="W27">
+        <v>22</v>
+      </c>
+      <c r="X27">
+        <v>23</v>
+      </c>
+      <c r="Y27">
+        <v>24</v>
+      </c>
+      <c r="Z27">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>